<commit_message>
refactoring and import merge
</commit_message>
<xml_diff>
--- a/ImportService/App_Data/PBTest.xlsx
+++ b/ImportService/App_Data/PBTest.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="155">
   <si>
     <t>ABEGOUCH</t>
   </si>
@@ -483,6 +483,15 @@
   </si>
   <si>
     <t>200-250 CM RB</t>
+  </si>
+  <si>
+    <t>Barry Hebbron</t>
+  </si>
+  <si>
+    <t>152CM</t>
+  </si>
+  <si>
+    <t>BDHNEW</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100:XFD29843"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3596,6 +3605,52 @@
         <v>43525</v>
       </c>
     </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>5000</v>
+      </c>
+      <c r="B100" t="s">
+        <v>127</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D100" t="s">
+        <v>128</v>
+      </c>
+      <c r="E100" t="s">
+        <v>151</v>
+      </c>
+      <c r="F100">
+        <v>100</v>
+      </c>
+      <c r="G100" s="1">
+        <v>43511</v>
+      </c>
+      <c r="H100" s="1">
+        <v>43525</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>3000</v>
+      </c>
+      <c r="B101" t="s">
+        <v>154</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D101" t="s">
+        <v>152</v>
+      </c>
+      <c r="E101" t="s">
+        <v>153</v>
+      </c>
+      <c r="F101">
+        <v>2000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>